<commit_message>
🐷 Bigger fonts for graphics
</commit_message>
<xml_diff>
--- a/Homework1/Task3/graphics/Task3_Diagramme.xlsx
+++ b/Homework1/Task3/graphics/Task3_Diagramme.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bee/Documents/__FH/FH Salzburg/02_Recommender_Systems/02_Homework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bee/Documents/__FH/FH Salzburg/02_Recommender_Systems/02_Homework/01/recommender-systems/Homework1/Task3/graphics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task3 Unser CF" sheetId="1" r:id="rId1"/>
@@ -317,13 +317,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -331,13 +325,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -356,6 +344,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -396,7 +396,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -409,14 +409,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" b="1"/>
+              <a:rPr lang="de-DE" sz="2400" b="1"/>
               <a:t>UNSER</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="de-DE" b="1" baseline="0"/>
+              <a:rPr lang="de-DE" sz="2400" b="1" baseline="0"/>
               <a:t> CF</a:t>
             </a:r>
-            <a:endParaRPr lang="de-DE" b="1"/>
+            <a:endParaRPr lang="de-DE" sz="2400" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -434,7 +434,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -739,7 +739,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="l"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -747,11 +746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098154464"/>
-        <c:axId val="-2081452992"/>
+        <c:axId val="2138754512"/>
+        <c:axId val="2117112496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098154464"/>
+        <c:axId val="2138754512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -778,7 +777,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -791,16 +790,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:rPr lang="de-DE" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
                   <a:t>Neighbours</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                   <a:t> </a:t>
                 </a:r>
-                <a:endParaRPr lang="de-DE" sz="1200" b="1"/>
+                <a:endParaRPr lang="de-DE" sz="2000" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -818,7 +817,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -855,7 +854,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -870,12 +869,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2081452992"/>
+        <c:crossAx val="2117112496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2081452992"/>
+        <c:axId val="2117112496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +901,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -915,7 +914,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>Prozent</a:t>
                 </a:r>
               </a:p>
@@ -935,7 +934,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -973,7 +972,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -988,7 +987,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098154464"/>
+        <c:crossAx val="2138754512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1016,7 +1015,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1090,7 +1089,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1103,7 +1102,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" b="1"/>
+              <a:rPr lang="de-DE" sz="2400" b="1"/>
               <a:t>RB RANDOM ARTISTS</a:t>
             </a:r>
           </a:p>
@@ -1123,7 +1122,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1435,11 +1434,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2082162432"/>
-        <c:axId val="-2082020320"/>
+        <c:axId val="2138800256"/>
+        <c:axId val="2138806240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2082162432"/>
+        <c:axId val="2138800256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1465,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1479,7 +1478,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>Artists</a:t>
                 </a:r>
               </a:p>
@@ -1499,7 +1498,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1536,7 +1535,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1551,12 +1550,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082020320"/>
+        <c:crossAx val="2138806240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2082020320"/>
+        <c:axId val="2138806240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,7 +1582,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1596,7 +1595,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>Prozent</a:t>
                 </a:r>
               </a:p>
@@ -1616,7 +1615,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1654,7 +1653,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1669,7 +1668,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082162432"/>
+        <c:crossAx val="2138800256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1697,7 +1696,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1771,7 +1770,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1784,7 +1783,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" b="1"/>
+              <a:rPr lang="de-DE" sz="2400" b="1"/>
               <a:t>RB USER PICK</a:t>
             </a:r>
           </a:p>
@@ -1804,7 +1803,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2116,11 +2115,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2058349488"/>
-        <c:axId val="-2028964288"/>
+        <c:axId val="2138848080"/>
+        <c:axId val="2138854064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2058349488"/>
+        <c:axId val="2138848080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,7 +2146,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2160,7 +2159,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>Artists</a:t>
                 </a:r>
               </a:p>
@@ -2180,7 +2179,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2217,7 +2216,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2232,12 +2231,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028964288"/>
+        <c:crossAx val="2138854064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028964288"/>
+        <c:axId val="2138854064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2264,7 +2263,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2277,7 +2276,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>Prozent</a:t>
                 </a:r>
               </a:p>
@@ -2297,7 +2296,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2335,7 +2334,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2350,7 +2349,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058349488"/>
+        <c:crossAx val="2138848080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2378,7 +2377,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2452,7 +2451,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2465,7 +2464,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" b="1"/>
+              <a:rPr lang="de-DE" sz="2400" b="1"/>
               <a:t>VERGLEICH VERSCHIEDENER RECOMMENDER</a:t>
             </a:r>
           </a:p>
@@ -2485,7 +2484,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2797,11 +2796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2059891552"/>
-        <c:axId val="-2083714800"/>
+        <c:axId val="-2121944672"/>
+        <c:axId val="-2121938576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2059891552"/>
+        <c:axId val="-2121944672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2828,7 +2827,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2841,7 +2840,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>MAR %</a:t>
                 </a:r>
               </a:p>
@@ -2861,7 +2860,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2899,7 +2898,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2914,12 +2913,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083714800"/>
+        <c:crossAx val="-2121938576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2083714800"/>
+        <c:axId val="-2121938576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2946,7 +2945,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2959,7 +2958,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1200" b="1"/>
+                  <a:rPr lang="de-DE" sz="2000" b="1"/>
                   <a:t>MAP %</a:t>
                 </a:r>
               </a:p>
@@ -2979,7 +2978,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3017,7 +3016,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3032,7 +3031,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059891552"/>
+        <c:crossAx val="-2121944672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3060,7 +3059,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5750,8 +5749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5762,12 +5761,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -5880,19 +5879,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -6012,12 +6011,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -6118,7 +6117,7 @@
       </c>
     </row>
     <row r="18" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L18" s="23"/>
+      <c r="L18" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6134,48 +6133,48 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="9">
         <v>2.59</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>1.05</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="10">
         <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -6185,12 +6184,12 @@
       <c r="D3" s="3">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>1.6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -6200,12 +6199,12 @@
       <c r="D4" s="3">
         <v>1.19</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>1.69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="4">
         <v>5</v>
       </c>
@@ -6215,12 +6214,12 @@
       <c r="D5" s="3">
         <v>1.2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>1.71</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4">
         <v>10</v>
       </c>
@@ -6230,44 +6229,44 @@
       <c r="D6" s="3">
         <v>1.26</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>1.79</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16">
+      <c r="A7" s="23"/>
+      <c r="B7" s="12">
         <v>20</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="13">
         <v>3.24</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="13">
         <v>1.34</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="14">
         <v>1.89</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.22</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0.01</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4">
         <v>5</v>
       </c>
@@ -6277,12 +6276,12 @@
       <c r="D9" s="3">
         <v>0.04</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <v>0.08</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4">
         <v>10</v>
       </c>
@@ -6292,12 +6291,12 @@
       <c r="D10" s="3">
         <v>0.09</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="11">
         <v>0.13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4">
         <v>20</v>
       </c>
@@ -6307,12 +6306,12 @@
       <c r="D11" s="3">
         <v>0.2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>0.24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4">
         <v>50</v>
       </c>
@@ -6322,44 +6321,44 @@
       <c r="D12" s="3">
         <v>0.49</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="11">
         <v>0.39</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16">
+      <c r="A13" s="23"/>
+      <c r="B13" s="12">
         <v>100</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="13">
         <v>0.32</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="13">
         <v>1.04</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="14">
         <v>0.49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="9">
         <v>0.85</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>0.02</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4">
         <v>5</v>
       </c>
@@ -6369,12 +6368,12 @@
       <c r="D15" s="3">
         <v>0.15</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="4">
         <v>10</v>
       </c>
@@ -6384,12 +6383,12 @@
       <c r="D16" s="3">
         <v>0.31</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="11">
         <v>0.44</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="4">
         <v>20</v>
       </c>
@@ -6399,12 +6398,12 @@
       <c r="D17" s="3">
         <v>0.54</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="11">
         <v>0.66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="4">
         <v>50</v>
       </c>
@@ -6414,22 +6413,22 @@
       <c r="D18" s="3">
         <v>0.98</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="11">
         <v>0.85</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16">
+      <c r="A19" s="23"/>
+      <c r="B19" s="12">
         <v>100</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="13">
         <v>0.8</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="13">
         <v>1.99</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed sizing at comparison_all File
</commit_message>
<xml_diff>
--- a/Homework1/Task3/graphics/Task3_Diagramme.xlsx
+++ b/Homework1/Task3/graphics/Task3_Diagramme.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Task3 Unser CF" sheetId="1" r:id="rId1"/>
@@ -5451,16 +5451,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>170180</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>649243</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5879,8 +5879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6005,7 +6005,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D8"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6132,8 +6132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>